<commit_message>
creacion de la tabla condensadoras con los cotones añadir,modificar y eliminar, modificando tambien los parametros para crear los filtros.
</commit_message>
<xml_diff>
--- a/src/main/resources/datos/Inventario AA V2.xlsx
+++ b/src/main/resources/datos/Inventario AA V2.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="233">
   <si>
     <t xml:space="preserve">Cuenta de Planta</t>
   </si>
@@ -754,6 +754,9 @@
   </si>
   <si>
     <t xml:space="preserve">MARCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOSHIBA</t>
   </si>
   <si>
     <t xml:space="preserve">MODELO</t>
@@ -771,7 +774,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -844,6 +847,12 @@
       <name val="Aptos"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1099,7 +1108,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1334,6 +1343,10 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1753,9 +1766,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>59760</xdr:colOff>
+      <xdr:colOff>59040</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1769,7 +1782,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="679320" y="1638000"/>
-          <a:ext cx="7388280" cy="4093200"/>
+          <a:ext cx="7387560" cy="4092480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6752,20 +6765,65 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="59" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="59" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="59" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="59" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="59" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="59" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="59" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="59" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="59" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -6816,17 +6874,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>231</v>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="59" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="59" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="59" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="59" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -11516,13 +11594,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11941,7 +12019,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="49" t="s">
         <v>90</v>
       </c>
@@ -12209,7 +12287,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="49" t="s">
         <v>104</v>
       </c>
@@ -12321,7 +12399,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="35" t="s">
         <v>111</v>
       </c>
@@ -12374,7 +12452,7 @@
         <v>45506</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="35" t="s">
         <v>120</v>
       </c>
@@ -12539,6 +12617,11 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:I33">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="ACTIVO"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:I33">
       <sortCondition ref="A2:A33" customList=""/>
     </sortState>
@@ -12792,10 +12875,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12809,6 +12892,26 @@
       </c>
       <c r="B1" s="38" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="59" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="59" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="59" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="59" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -12868,10 +12971,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12882,6 +12985,16 @@
       </c>
       <c r="B1" s="38" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="59" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -12910,7 +13023,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>228</v>

</xml_diff>